<commit_message>
Added support for islamic countries
</commit_message>
<xml_diff>
--- a/coin_sample.xlsx
+++ b/coin_sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="63">
   <si>
     <t xml:space="preserve">Japan</t>
   </si>
@@ -89,6 +89,126 @@
   </si>
   <si>
     <t xml:space="preserve">Y# 568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Baisa - Qaboos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Baisa - Qaboos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 45a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Baisa - Qaboos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 152a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Baisa - Qaboos (magnetic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Baisa - Qaboos (National Day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Baisa - Qaboos (United Nations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Baisa - Qaboos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 153a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Baisa - Qaboos (magnetic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Baisa - Qaboos (National Day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Dīnār - Rezā Pahlavī</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1171a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Rial - Mohammad Rezā Pahlavī</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Rial - Mohammad Rezā Pahlavī</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1175a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Rial - Mohammad Rezā Pahlavī</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Rial - Mohammad Rezā Pahlavī</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Rial (Oil and Agriculture)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 1271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 Rial (Saadi Tomb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iraq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 126a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Fils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM# 128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Fils</t>
   </si>
 </sst>
 </file>
@@ -196,18 +316,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G87" activeCellId="0" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
     <col collapsed="false" hidden="true" max="3" min="3" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,49 +1419,725 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>1400</v>
+      </c>
+    </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1733,6 +2530,49 @@
     <hyperlink ref="C62" r:id="rId62" display="»"/>
     <hyperlink ref="C63" r:id="rId63" display="»"/>
     <hyperlink ref="C64" r:id="rId64" display="»"/>
+    <hyperlink ref="C65" r:id="rId65" display="»"/>
+    <hyperlink ref="C66" r:id="rId66" display="»"/>
+    <hyperlink ref="C67" r:id="rId67" display="»"/>
+    <hyperlink ref="C68" r:id="rId68" display="»"/>
+    <hyperlink ref="C69" r:id="rId69" display="»"/>
+    <hyperlink ref="C70" r:id="rId70" display="»"/>
+    <hyperlink ref="C71" r:id="rId71" display="»"/>
+    <hyperlink ref="C72" r:id="rId72" display="»"/>
+    <hyperlink ref="C73" r:id="rId73" display="»"/>
+    <hyperlink ref="C74" r:id="rId74" display="»"/>
+    <hyperlink ref="C75" r:id="rId75" display="»"/>
+    <hyperlink ref="C76" r:id="rId76" display="»"/>
+    <hyperlink ref="C77" r:id="rId77" display="»"/>
+    <hyperlink ref="C78" r:id="rId78" display="»"/>
+    <hyperlink ref="C79" r:id="rId79" display="»"/>
+    <hyperlink ref="C80" r:id="rId80" display="»"/>
+    <hyperlink ref="C81" r:id="rId81" display="»"/>
+    <hyperlink ref="C82" r:id="rId82" display="»"/>
+    <hyperlink ref="C83" r:id="rId83" display="»"/>
+    <hyperlink ref="C84" r:id="rId84" display="»"/>
+    <hyperlink ref="C85" r:id="rId85" display="»"/>
+    <hyperlink ref="C86" r:id="rId86" display="»"/>
+    <hyperlink ref="C87" r:id="rId87" display="»"/>
+    <hyperlink ref="C88" r:id="rId88" display="»"/>
+    <hyperlink ref="C89" r:id="rId89" display="»"/>
+    <hyperlink ref="C90" r:id="rId90" display="»"/>
+    <hyperlink ref="C91" r:id="rId91" display="»"/>
+    <hyperlink ref="C92" r:id="rId92" display="»"/>
+    <hyperlink ref="C93" r:id="rId93" display="»"/>
+    <hyperlink ref="C94" r:id="rId94" display="»"/>
+    <hyperlink ref="C95" r:id="rId95" display="»"/>
+    <hyperlink ref="C96" r:id="rId96" display="»"/>
+    <hyperlink ref="C97" r:id="rId97" display="»"/>
+    <hyperlink ref="C98" r:id="rId98" display="»"/>
+    <hyperlink ref="C99" r:id="rId99" display="»"/>
+    <hyperlink ref="C100" r:id="rId100" display="»"/>
+    <hyperlink ref="C101" r:id="rId101" display="»"/>
+    <hyperlink ref="C102" r:id="rId102" display="»"/>
+    <hyperlink ref="C103" r:id="rId103" display="»"/>
+    <hyperlink ref="C104" r:id="rId104" display="»"/>
+    <hyperlink ref="C105" r:id="rId105" display="»"/>
+    <hyperlink ref="C106" r:id="rId106" display="»"/>
+    <hyperlink ref="C107" r:id="rId107" display="»"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>